<commit_message>
Tabela de Dados em Teste de hipóteses
</commit_message>
<xml_diff>
--- a/Otimização+e+Metas.xlsx
+++ b/Otimização+e+Metas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMAN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMAN\Desktop\Curso-Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41A3CD8-6D76-4E49-83D5-34B897E7E5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F15CB39-8C49-4601-AF5A-B09009BACF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="2" r:id="rId1"/>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Revendedora João&amp;Co</t>
   </si>
@@ -195,16 +195,21 @@
   </si>
   <si>
     <t>Lucro antes de despesas</t>
+  </si>
+  <si>
+    <t>Volume</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +238,13 @@
       <name val="Segoe UI"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -388,10 +400,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -434,9 +447,11 @@
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -716,7 +731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -792,71 +807,362 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:C9"/>
+  <dimension ref="B2:M20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E4" s="28">
+        <f>C4*C5*C6</f>
+        <v>345000</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>21</v>
       </c>
       <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>20</v>
+      </c>
+      <c r="F5" s="28">
+        <f t="dataTable" ref="F5:H10" dt2D="1" dtr="1" r1="C4" r2="C5"/>
+        <v>300000</v>
+      </c>
+      <c r="G5" s="28">
+        <v>600000</v>
+      </c>
+      <c r="H5" s="28">
+        <v>900000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="15">
         <v>15000</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E6" s="3">
+        <v>21</v>
+      </c>
+      <c r="F6" s="28">
+        <v>315000</v>
+      </c>
+      <c r="G6" s="28">
+        <v>630000</v>
+      </c>
+      <c r="H6" s="28">
+        <v>945000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="14">
         <v>3500</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E7" s="3">
+        <v>22</v>
+      </c>
+      <c r="F7" s="28">
+        <v>330000</v>
+      </c>
+      <c r="G7" s="28">
+        <v>660000</v>
+      </c>
+      <c r="H7" s="28">
+        <v>990000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="15">
         <f>C6*C5*C4</f>
-        <v>600000</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+        <v>345000</v>
+      </c>
+      <c r="E8" s="3">
+        <v>23</v>
+      </c>
+      <c r="F8" s="28">
+        <v>345000</v>
+      </c>
+      <c r="G8" s="28">
+        <v>690000</v>
+      </c>
+      <c r="H8" s="28">
+        <v>1035000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="14">
         <f>C7*C5*C4</f>
+        <v>80500</v>
+      </c>
+      <c r="E9" s="3">
+        <v>24</v>
+      </c>
+      <c r="F9" s="28">
+        <v>360000</v>
+      </c>
+      <c r="G9" s="28">
+        <v>720000</v>
+      </c>
+      <c r="H9" s="28">
+        <v>1080000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E10" s="3">
+        <v>25</v>
+      </c>
+      <c r="F10" s="28">
+        <v>375000</v>
+      </c>
+      <c r="G10" s="28">
+        <v>750000</v>
+      </c>
+      <c r="H10" s="28">
+        <v>1125000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E14" s="6">
+        <f>C4*C5*C7</f>
+        <v>80500</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>2</v>
+      </c>
+      <c r="H14" s="3">
+        <v>3</v>
+      </c>
+      <c r="J14" s="6">
+        <f>C4*C5*C7</f>
+        <v>80500</v>
+      </c>
+      <c r="K14" s="3">
+        <v>1</v>
+      </c>
+      <c r="L14" s="3">
+        <v>2</v>
+      </c>
+      <c r="M14" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E15" s="3">
+        <v>20</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="dataTable" ref="F15:H20" dt2D="1" dtr="1" r1="C4" r2="C5" ca="1"/>
+        <v>70000</v>
+      </c>
+      <c r="G15" s="3">
         <v>140000</v>
+      </c>
+      <c r="H15" s="3">
+        <v>210000</v>
+      </c>
+      <c r="J15" s="3">
+        <v>24</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="dataTable" ref="K15:M20" dt2D="1" dtr="1" r1="C4" r2="C5" ca="1"/>
+        <v>84000</v>
+      </c>
+      <c r="L15" s="3">
+        <v>168000</v>
+      </c>
+      <c r="M15" s="3">
+        <v>252000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E16" s="3">
+        <v>21</v>
+      </c>
+      <c r="F16" s="3">
+        <v>73500</v>
+      </c>
+      <c r="G16" s="3">
+        <v>147000</v>
+      </c>
+      <c r="H16" s="3">
+        <v>220500</v>
+      </c>
+      <c r="J16" s="3">
+        <v>25</v>
+      </c>
+      <c r="K16" s="3">
+        <v>87500</v>
+      </c>
+      <c r="L16" s="3">
+        <v>175000</v>
+      </c>
+      <c r="M16" s="3">
+        <v>262500</v>
+      </c>
+    </row>
+    <row r="17" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E17" s="3">
+        <v>22</v>
+      </c>
+      <c r="F17" s="3">
+        <v>77000</v>
+      </c>
+      <c r="G17" s="3">
+        <v>154000</v>
+      </c>
+      <c r="H17" s="3">
+        <v>231000</v>
+      </c>
+      <c r="J17" s="3">
+        <v>26</v>
+      </c>
+      <c r="K17" s="3">
+        <v>91000</v>
+      </c>
+      <c r="L17" s="3">
+        <v>182000</v>
+      </c>
+      <c r="M17" s="3">
+        <v>273000</v>
+      </c>
+    </row>
+    <row r="18" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E18" s="3">
+        <v>23</v>
+      </c>
+      <c r="F18" s="3">
+        <v>80500</v>
+      </c>
+      <c r="G18" s="3">
+        <v>161000</v>
+      </c>
+      <c r="H18" s="3">
+        <v>241500</v>
+      </c>
+      <c r="J18" s="3">
+        <v>27</v>
+      </c>
+      <c r="K18" s="3">
+        <v>94500</v>
+      </c>
+      <c r="L18" s="3">
+        <v>189000</v>
+      </c>
+      <c r="M18" s="3">
+        <v>283500</v>
+      </c>
+    </row>
+    <row r="19" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E19" s="3">
+        <v>24</v>
+      </c>
+      <c r="F19" s="3">
+        <v>84000</v>
+      </c>
+      <c r="G19" s="3">
+        <v>168000</v>
+      </c>
+      <c r="H19" s="3">
+        <v>252000</v>
+      </c>
+      <c r="J19" s="3">
+        <v>28</v>
+      </c>
+      <c r="K19" s="3">
+        <v>98000</v>
+      </c>
+      <c r="L19" s="3">
+        <v>196000</v>
+      </c>
+      <c r="M19" s="3">
+        <v>294000</v>
+      </c>
+    </row>
+    <row r="20" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E20" s="3">
+        <v>25</v>
+      </c>
+      <c r="F20" s="3">
+        <v>87500</v>
+      </c>
+      <c r="G20" s="3">
+        <v>175000</v>
+      </c>
+      <c r="H20" s="3">
+        <v>262500</v>
+      </c>
+      <c r="J20" s="3">
+        <v>29</v>
+      </c>
+      <c r="K20" s="3">
+        <v>101500</v>
+      </c>
+      <c r="L20" s="3">
+        <v>203000</v>
+      </c>
+      <c r="M20" s="3">
+        <v>304500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solver - Pesquisa Operacional
</commit_message>
<xml_diff>
--- a/Otimização+e+Metas.xlsx
+++ b/Otimização+e+Metas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMAN\Desktop\Curso-Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F15CB39-8C49-4601-AF5A-B09009BACF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05510375-A066-4B1A-BE52-64177A577B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="2" hidden="1">número inteiro</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">"número inteiro"</definedName>
     <definedName name="solver_rhs2" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs3" localSheetId="2" hidden="1">Solver!$C$11</definedName>
     <definedName name="solver_rhs4" localSheetId="2" hidden="1">Solver!$C$12</definedName>
@@ -101,6 +101,112 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>AMAN</author>
+  </authors>
+  <commentList>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{44E95470-A5C8-4AAB-8D9E-1EF6E5E8E666}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>AMAN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Tabela de dados com Teste de Hopóteses</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{DA3D8FEF-46E0-4D1C-A51B-7AA15B968D49}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">AMAN:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Aqui fica qual a fórmula vamos utilizar</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{D935EA47-0A0A-4C87-92CF-78AACDE14567}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>AMAN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Aqui fica qual dado substituir na fórmula para testar as hipóteses - Substituindo o c5</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{921CDD1E-FEFB-46DE-9FA8-17EE27F61902}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>AMAN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Aqui fica qual dado substituir na fórmula para testar as hipóteses - Substituindo o c4 de dentro da fórmula</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
@@ -207,9 +313,9 @@
   <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,8 +351,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +375,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -404,7 +541,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -439,15 +576,18 @@
     <xf numFmtId="8" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -806,11 +946,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:M20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,7 +980,7 @@
       <c r="C4">
         <v>23</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="24">
         <f>C4*C5*C6</f>
         <v>345000</v>
       </c>
@@ -864,14 +1004,14 @@
       <c r="E5" s="3">
         <v>20</v>
       </c>
-      <c r="F5" s="28">
-        <f t="dataTable" ref="F5:H10" dt2D="1" dtr="1" r1="C4" r2="C5"/>
+      <c r="F5" s="24">
+        <f t="dataTable" ref="F5:H10" dt2D="1" dtr="1" r1="C4" r2="C5" ca="1"/>
         <v>300000</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="24">
         <v>600000</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="24">
         <v>900000</v>
       </c>
     </row>
@@ -885,13 +1025,13 @@
       <c r="E6" s="3">
         <v>21</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="24">
         <v>315000</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="24">
         <v>630000</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="24">
         <v>945000</v>
       </c>
     </row>
@@ -905,13 +1045,13 @@
       <c r="E7" s="3">
         <v>22</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="24">
         <v>330000</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="24">
         <v>660000</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="24">
         <v>990000</v>
       </c>
     </row>
@@ -926,13 +1066,13 @@
       <c r="E8" s="3">
         <v>23</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="24">
         <v>345000</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="24">
         <v>690000</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="24">
         <v>1035000</v>
       </c>
     </row>
@@ -947,13 +1087,13 @@
       <c r="E9" s="3">
         <v>24</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="24">
         <v>360000</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="24">
         <v>720000</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="24">
         <v>1080000</v>
       </c>
     </row>
@@ -961,13 +1101,13 @@
       <c r="E10" s="3">
         <v>25</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="24">
         <v>375000</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="24">
         <v>750000</v>
       </c>
-      <c r="H10" s="28">
+      <c r="H10" s="24">
         <v>1125000</v>
       </c>
     </row>
@@ -1012,7 +1152,7 @@
         <v>20</v>
       </c>
       <c r="F15" s="3">
-        <f t="dataTable" ref="F15:H20" dt2D="1" dtr="1" r1="C4" r2="C5" ca="1"/>
+        <f t="dataTable" ref="F15:H20" dt2D="1" dtr="1" r1="C4" r2="C5"/>
         <v>70000</v>
       </c>
       <c r="G15" s="3">
@@ -1167,22 +1307,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:J12"/>
+  <dimension ref="B1:J16"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
@@ -1243,10 +1384,21 @@
       <c r="F5" s="10">
         <v>1</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="3"/>
+      <c r="G5" s="4">
+        <v>51</v>
+      </c>
+      <c r="H5" s="6">
+        <f>G5*C5</f>
+        <v>148410</v>
+      </c>
+      <c r="I5" s="6">
+        <f>G5*E5</f>
+        <v>77265</v>
+      </c>
+      <c r="J5" s="3">
+        <f>G5*F5</f>
+        <v>51</v>
+      </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -1265,10 +1417,21 @@
       <c r="F6" s="10">
         <v>0.3</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="3"/>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6">
+        <f t="shared" ref="H6:H7" si="1">G6*C6</f>
+        <v>1000</v>
+      </c>
+      <c r="I6" s="6">
+        <f t="shared" ref="I6:I7" si="2">G6*E6</f>
+        <v>500</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" ref="J6:J7" si="3">G6*F6</f>
+        <v>0.3</v>
+      </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
@@ -1287,10 +1450,21 @@
       <c r="F7" s="10">
         <v>0.5</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="3"/>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
@@ -1301,31 +1475,31 @@
         <v>5610</v>
       </c>
       <c r="D9" s="5">
-        <f t="shared" ref="D9:J9" si="1">SUM(D5:D7)</f>
+        <f t="shared" ref="D9:J9" si="4">SUM(D5:D7)</f>
         <v>8425</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2815</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>52</v>
+      </c>
+      <c r="H9" s="25">
+        <f t="shared" si="4"/>
+        <v>149410</v>
+      </c>
+      <c r="I9" s="27">
+        <f t="shared" si="4"/>
+        <v>77765</v>
+      </c>
+      <c r="J9" s="28">
+        <f t="shared" si="4"/>
+        <v>51.3</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
@@ -1340,12 +1514,18 @@
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="29">
         <v>100</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
       </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>